<commit_message>
Script for auto placing.
</commit_message>
<xml_diff>
--- a/practice_programs/Electro_suply/data.xlsx
+++ b/practice_programs/Electro_suply/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Programmpractice work\practice-work\practice_programs\Electro_suply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBFA247-8A1F-44FE-B184-815EEB18B274}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6567C64-FD65-4D9F-95BD-0BE401A7602F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1590" windowWidth="28800" windowHeight="14610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3525" yWindow="4305" windowWidth="28800" windowHeight="14610" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Pуст</t>
   </si>
@@ -49,6 +49,30 @@
   </si>
   <si>
     <t>Pуд</t>
+  </si>
+  <si>
+    <t>Pp</t>
+  </si>
+  <si>
+    <t>Qp</t>
+  </si>
+  <si>
+    <t>Pno</t>
+  </si>
+  <si>
+    <t>Ppo</t>
+  </si>
+  <si>
+    <t>Ppsum</t>
+  </si>
+  <si>
+    <t>Qpsum</t>
+  </si>
+  <si>
+    <t>Spsum</t>
+  </si>
+  <si>
+    <t>tg</t>
   </si>
 </sst>
 </file>
@@ -368,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="A1:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,14 +765,777 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4517EC5B-3670-41CB-88A1-BD71DE1561D0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1720</v>
+      </c>
+      <c r="C2">
+        <v>0.4</v>
+      </c>
+      <c r="D2">
+        <v>0.75</v>
+      </c>
+      <c r="E2">
+        <v>0.88</v>
+      </c>
+      <c r="F2">
+        <v>688</v>
+      </c>
+      <c r="G2">
+        <v>606.76</v>
+      </c>
+      <c r="H2">
+        <v>1211</v>
+      </c>
+      <c r="I2">
+        <v>18</v>
+      </c>
+      <c r="J2">
+        <v>21.8</v>
+      </c>
+      <c r="K2">
+        <v>0.95</v>
+      </c>
+      <c r="L2">
+        <v>20.71</v>
+      </c>
+      <c r="M2">
+        <v>708.71</v>
+      </c>
+      <c r="N2">
+        <v>606.76</v>
+      </c>
+      <c r="O2">
+        <v>932.96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1660</v>
+      </c>
+      <c r="C3">
+        <v>0.35</v>
+      </c>
+      <c r="D3">
+        <v>0.8</v>
+      </c>
+      <c r="E3">
+        <v>0.75</v>
+      </c>
+      <c r="F3">
+        <v>581</v>
+      </c>
+      <c r="G3">
+        <v>435.75</v>
+      </c>
+      <c r="H3">
+        <v>1406.25</v>
+      </c>
+      <c r="I3">
+        <v>18</v>
+      </c>
+      <c r="J3">
+        <v>25.31</v>
+      </c>
+      <c r="K3">
+        <v>0.95</v>
+      </c>
+      <c r="L3">
+        <v>24.05</v>
+      </c>
+      <c r="M3">
+        <v>605.04999999999995</v>
+      </c>
+      <c r="N3">
+        <v>435.75</v>
+      </c>
+      <c r="O3">
+        <v>745.63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1050</v>
+      </c>
+      <c r="C4">
+        <v>0.7</v>
+      </c>
+      <c r="D4">
+        <v>0.65</v>
+      </c>
+      <c r="E4">
+        <v>1.17</v>
+      </c>
+      <c r="F4">
+        <v>735</v>
+      </c>
+      <c r="G4">
+        <v>859.31</v>
+      </c>
+      <c r="H4">
+        <v>234.4</v>
+      </c>
+      <c r="I4">
+        <v>16</v>
+      </c>
+      <c r="J4">
+        <v>3.75</v>
+      </c>
+      <c r="K4">
+        <v>0.85</v>
+      </c>
+      <c r="L4">
+        <v>3.19</v>
+      </c>
+      <c r="M4">
+        <v>738.19</v>
+      </c>
+      <c r="N4">
+        <v>859.31</v>
+      </c>
+      <c r="O4">
+        <v>1132.8399999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>830</v>
+      </c>
+      <c r="C5">
+        <v>0.3</v>
+      </c>
+      <c r="D5">
+        <v>0.65</v>
+      </c>
+      <c r="E5">
+        <v>1.17</v>
+      </c>
+      <c r="F5">
+        <v>249</v>
+      </c>
+      <c r="G5">
+        <v>291.11</v>
+      </c>
+      <c r="H5">
+        <v>1953.1</v>
+      </c>
+      <c r="I5">
+        <v>17</v>
+      </c>
+      <c r="J5">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="K5">
+        <v>0.85</v>
+      </c>
+      <c r="L5">
+        <v>28.22</v>
+      </c>
+      <c r="M5">
+        <v>277.22000000000003</v>
+      </c>
+      <c r="N5">
+        <v>291.11</v>
+      </c>
+      <c r="O5">
+        <v>401.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1120</v>
+      </c>
+      <c r="C6">
+        <v>0.3</v>
+      </c>
+      <c r="D6">
+        <v>0.7</v>
+      </c>
+      <c r="E6">
+        <v>1.02</v>
+      </c>
+      <c r="F6">
+        <v>336</v>
+      </c>
+      <c r="G6">
+        <v>342.79</v>
+      </c>
+      <c r="H6">
+        <v>2617.1999999999998</v>
+      </c>
+      <c r="I6">
+        <v>18</v>
+      </c>
+      <c r="J6">
+        <v>47.11</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>47.11</v>
+      </c>
+      <c r="M6">
+        <v>383.11</v>
+      </c>
+      <c r="N6">
+        <v>342.79</v>
+      </c>
+      <c r="O6">
+        <v>514.08000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>740</v>
+      </c>
+      <c r="C7">
+        <v>0.35</v>
+      </c>
+      <c r="D7">
+        <v>0.7</v>
+      </c>
+      <c r="E7">
+        <v>1.02</v>
+      </c>
+      <c r="F7">
+        <v>259</v>
+      </c>
+      <c r="G7">
+        <v>264.23</v>
+      </c>
+      <c r="H7">
+        <v>546.87</v>
+      </c>
+      <c r="I7">
+        <v>18</v>
+      </c>
+      <c r="J7">
+        <v>9.84</v>
+      </c>
+      <c r="K7">
+        <v>0.95</v>
+      </c>
+      <c r="L7">
+        <v>9.35</v>
+      </c>
+      <c r="M7">
+        <v>268.35000000000002</v>
+      </c>
+      <c r="N7">
+        <v>264.23</v>
+      </c>
+      <c r="O7">
+        <v>376.61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>600</v>
+      </c>
+      <c r="C8">
+        <v>0.3</v>
+      </c>
+      <c r="D8">
+        <v>0.7</v>
+      </c>
+      <c r="E8">
+        <v>1.02</v>
+      </c>
+      <c r="F8">
+        <v>180</v>
+      </c>
+      <c r="G8">
+        <v>183.64</v>
+      </c>
+      <c r="H8">
+        <v>625</v>
+      </c>
+      <c r="I8">
+        <v>18</v>
+      </c>
+      <c r="J8">
+        <v>11.25</v>
+      </c>
+      <c r="K8">
+        <v>0.95</v>
+      </c>
+      <c r="L8">
+        <v>10.69</v>
+      </c>
+      <c r="M8">
+        <v>190.69</v>
+      </c>
+      <c r="N8">
+        <v>183.64</v>
+      </c>
+      <c r="O8">
+        <v>264.73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1630</v>
+      </c>
+      <c r="C9">
+        <v>0.7</v>
+      </c>
+      <c r="D9">
+        <v>0.8</v>
+      </c>
+      <c r="E9">
+        <v>0.75</v>
+      </c>
+      <c r="F9">
+        <v>1141</v>
+      </c>
+      <c r="G9">
+        <v>855.75</v>
+      </c>
+      <c r="H9">
+        <v>1796.9</v>
+      </c>
+      <c r="I9">
+        <v>15</v>
+      </c>
+      <c r="J9">
+        <v>26.95</v>
+      </c>
+      <c r="K9">
+        <v>0.6</v>
+      </c>
+      <c r="L9">
+        <v>16.170000000000002</v>
+      </c>
+      <c r="M9">
+        <v>1157.17</v>
+      </c>
+      <c r="N9">
+        <v>855.75</v>
+      </c>
+      <c r="O9">
+        <v>1439.22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>640</v>
+      </c>
+      <c r="C10">
+        <v>0.3</v>
+      </c>
+      <c r="D10">
+        <v>0.7</v>
+      </c>
+      <c r="E10">
+        <v>1.02</v>
+      </c>
+      <c r="F10">
+        <v>192</v>
+      </c>
+      <c r="G10">
+        <v>195.88</v>
+      </c>
+      <c r="H10">
+        <v>1796.9</v>
+      </c>
+      <c r="I10">
+        <v>18</v>
+      </c>
+      <c r="J10">
+        <v>32.340000000000003</v>
+      </c>
+      <c r="K10">
+        <v>0.95</v>
+      </c>
+      <c r="L10">
+        <v>30.73</v>
+      </c>
+      <c r="M10">
+        <v>222.73</v>
+      </c>
+      <c r="N10">
+        <v>195.88</v>
+      </c>
+      <c r="O10">
+        <v>296.61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>240</v>
+      </c>
+      <c r="C11">
+        <v>0.35</v>
+      </c>
+      <c r="D11">
+        <v>0.8</v>
+      </c>
+      <c r="E11">
+        <v>0.75</v>
+      </c>
+      <c r="F11">
+        <v>84</v>
+      </c>
+      <c r="G11">
+        <v>63</v>
+      </c>
+      <c r="H11">
+        <v>3020.8</v>
+      </c>
+      <c r="I11">
+        <v>15</v>
+      </c>
+      <c r="J11">
+        <v>45.31</v>
+      </c>
+      <c r="K11">
+        <v>0.6</v>
+      </c>
+      <c r="L11">
+        <v>27.19</v>
+      </c>
+      <c r="M11">
+        <v>111.19</v>
+      </c>
+      <c r="N11">
+        <v>63</v>
+      </c>
+      <c r="O11">
+        <v>127.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>420</v>
+      </c>
+      <c r="C12">
+        <v>0.35</v>
+      </c>
+      <c r="D12">
+        <v>0.8</v>
+      </c>
+      <c r="E12">
+        <v>0.75</v>
+      </c>
+      <c r="F12">
+        <v>147</v>
+      </c>
+      <c r="G12">
+        <v>110.25</v>
+      </c>
+      <c r="H12">
+        <v>1562.5</v>
+      </c>
+      <c r="I12">
+        <v>15</v>
+      </c>
+      <c r="J12">
+        <v>23.44</v>
+      </c>
+      <c r="K12">
+        <v>0.6</v>
+      </c>
+      <c r="L12">
+        <v>14.06</v>
+      </c>
+      <c r="M12">
+        <v>161.06</v>
+      </c>
+      <c r="N12">
+        <v>110.25</v>
+      </c>
+      <c r="O12">
+        <v>195.18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1340</v>
+      </c>
+      <c r="C13">
+        <v>0.78</v>
+      </c>
+      <c r="D13">
+        <v>0.8</v>
+      </c>
+      <c r="E13">
+        <v>0.75</v>
+      </c>
+      <c r="F13">
+        <v>1045.2</v>
+      </c>
+      <c r="G13">
+        <v>783.9</v>
+      </c>
+      <c r="H13">
+        <v>703.1</v>
+      </c>
+      <c r="I13">
+        <v>15</v>
+      </c>
+      <c r="J13">
+        <v>10.55</v>
+      </c>
+      <c r="K13">
+        <v>0.85</v>
+      </c>
+      <c r="L13">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="M13">
+        <v>1054.1600000000001</v>
+      </c>
+      <c r="N13">
+        <v>783.9</v>
+      </c>
+      <c r="O13">
+        <v>1313.68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>510</v>
+      </c>
+      <c r="C14">
+        <v>0.3</v>
+      </c>
+      <c r="D14">
+        <v>0.8</v>
+      </c>
+      <c r="E14">
+        <v>0.75</v>
+      </c>
+      <c r="F14">
+        <v>153</v>
+      </c>
+      <c r="G14">
+        <v>114.75</v>
+      </c>
+      <c r="H14">
+        <v>937.5</v>
+      </c>
+      <c r="I14">
+        <v>15</v>
+      </c>
+      <c r="J14">
+        <v>14.06</v>
+      </c>
+      <c r="K14">
+        <v>0.9</v>
+      </c>
+      <c r="L14">
+        <v>12.66</v>
+      </c>
+      <c r="M14">
+        <v>165.66</v>
+      </c>
+      <c r="N14">
+        <v>114.75</v>
+      </c>
+      <c r="O14">
+        <v>201.52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>490</v>
+      </c>
+      <c r="C15">
+        <v>0.45</v>
+      </c>
+      <c r="D15">
+        <v>0.9</v>
+      </c>
+      <c r="E15">
+        <v>0.48</v>
+      </c>
+      <c r="F15">
+        <v>220.5</v>
+      </c>
+      <c r="G15">
+        <v>106.79</v>
+      </c>
+      <c r="H15">
+        <v>703.1</v>
+      </c>
+      <c r="I15">
+        <v>15</v>
+      </c>
+      <c r="J15">
+        <v>10.55</v>
+      </c>
+      <c r="K15">
+        <v>0.9</v>
+      </c>
+      <c r="L15">
+        <v>9.49</v>
+      </c>
+      <c r="M15">
+        <v>229.99</v>
+      </c>
+      <c r="N15">
+        <v>106.79</v>
+      </c>
+      <c r="O15">
+        <v>253.58</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f>SUM(B2:B15)</f>
+        <v>12990</v>
+      </c>
+      <c r="F17">
+        <f>SUM(F2:F15)</f>
+        <v>6010.7</v>
+      </c>
+      <c r="G17">
+        <f>SUM(G2:G15)</f>
+        <v>5213.9099999999989</v>
+      </c>
+      <c r="H17">
+        <f>SUM(H2:H15)</f>
+        <v>19114.619999999995</v>
+      </c>
+      <c r="I17">
+        <f>SUM(I2:I15)</f>
+        <v>231</v>
+      </c>
+      <c r="J17">
+        <f>SUM(J2:J15)</f>
+        <v>315.46000000000004</v>
+      </c>
+      <c r="L17">
+        <f>SUM(L2:L15)</f>
+        <v>262.58</v>
+      </c>
+      <c r="M17">
+        <f>SUM(M2:M15)</f>
+        <v>6273.2799999999988</v>
+      </c>
+      <c r="N17">
+        <f>SUM(N2:N15)</f>
+        <v>5213.9099999999989</v>
+      </c>
+      <c r="O17">
+        <f>SUM(O2:O15)</f>
+        <v>8196.4300000000021</v>
+      </c>
+    </row>
+    <row r="38" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>1620</v>
+      </c>
+      <c r="P38">
+        <f>H13</f>
+        <v>703.1</v>
+      </c>
+      <c r="Q38">
+        <v>0.78</v>
+      </c>
+      <c r="R38">
+        <v>0.9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>